<commit_message>
added data from Lab 5 - Electron Diffraction
</commit_message>
<xml_diff>
--- a/TimeTrack2170.xlsx
+++ b/TimeTrack2170.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7004FB08-1086-4C24-96C8-E1A6241B7C73}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB8D6C7-3814-44E6-8FDE-708675159AAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>2200-0100</t>
+  </si>
+  <si>
+    <t>[Wk 10] Monday 21.5.18</t>
+  </si>
+  <si>
+    <t>Lab Report 4</t>
+  </si>
+  <si>
+    <t>1100-1300</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,10 +600,18 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -663,7 +680,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUBTOTAL(109,C2:C20)</f>
-        <v>18.16</v>
+        <v>20.16</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>